<commit_message>
fix template 2 bugs
</commit_message>
<xml_diff>
--- a/assets/templates_excel/template2.xlsx
+++ b/assets/templates_excel/template2.xlsx
@@ -3,16 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{A239C5A1-4E0E-4716-8F74-2EF14BA7E4C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34AB969-26A8-460B-A906-D9D436711E4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice" sheetId="24" r:id="rId1"/>
-    <sheet name="About" sheetId="25" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Invoice!$A$1:$H$38</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Invoice!$A$1:$H$37</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -35,27 +34,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>[Company Name]</t>
   </si>
   <si>
     <t>INVOICE</t>
-  </si>
-  <si>
-    <t>[Street Address]</t>
-  </si>
-  <si>
-    <t>INVOICE TEMPLATES BY VERTEX42.COM</t>
-  </si>
-  <si>
-    <t>[City, ST  ZIP]</t>
-  </si>
-  <si>
-    <t>https://www.vertex42.com/ExcelTemplates/invoice-templates.html</t>
-  </si>
-  <si>
-    <t>Phone: (000) 000-0000</t>
   </si>
   <si>
     <t>INVOICE #</t>
@@ -67,37 +51,13 @@
     <t>BILL TO</t>
   </si>
   <si>
-    <t>CUSTOMER ID</t>
-  </si>
-  <si>
-    <t>TERMS</t>
-  </si>
-  <si>
-    <t>← You can change TERMS to DUE DATE and enter a date (usually 30 days after the invoice date)</t>
-  </si>
-  <si>
     <t>[Name]</t>
-  </si>
-  <si>
-    <t>Due Upon Receipt</t>
-  </si>
-  <si>
-    <t>HOW TO SEND AN INVOICE TO A CLIENT</t>
   </si>
   <si>
     <t>[Phone]</t>
   </si>
   <si>
-    <t>1) Save or Print the worksheet as a PDF</t>
-  </si>
-  <si>
     <t>[Email Address]</t>
-  </si>
-  <si>
-    <t>2) Save a copy of the invoice for your records</t>
-  </si>
-  <si>
-    <t>3) Email the PDF to the client</t>
   </si>
   <si>
     <t>DESCRIPTION</t>
@@ -112,31 +72,13 @@
     <t>AMOUNT</t>
   </si>
   <si>
-    <t>← The QTY is assumed to be 1 if it is left blank</t>
-  </si>
-  <si>
     <t>Thank you for your business!</t>
   </si>
   <si>
     <t>SUBTOTAL</t>
   </si>
   <si>
-    <t>TAX RATE</t>
-  </si>
-  <si>
-    <t>← Enter the appropriate tax rate</t>
-  </si>
-  <si>
-    <t>TAX</t>
-  </si>
-  <si>
     <t>TOTAL</t>
-  </si>
-  <si>
-    <t>← Change the currency by editing the cell format</t>
-  </si>
-  <si>
-    <t>← Enter a note such as "Paid in full. Thank you!" if this is a receipt</t>
   </si>
   <si>
     <t>If you have any questions about this invoice, please contact</t>
@@ -145,28 +87,24 @@
     <t>[Name, Phone, email@address.com]</t>
   </si>
   <si>
-    <t>← Remember to update this information, or delete these two rows.</t>
+    <t>DISCOUNT</t>
   </si>
   <si>
-    <t>About Vertex42</t>
+    <t>[Mobile]</t>
   </si>
   <si>
-    <t>Vertex42.com provides over 300 professionally designed spreadsheet templates for business, home, and education - most of which are free to download. Their collection includes a variety of calendars, planners, and schedules as well as personal finance spreadsheets for budgeting, debt reduction, and loan amortization.</t>
-  </si>
-  <si>
-    <t>Businesses will find invoices, time sheets, inventory trackers, financial statements, and project planning templates. Teachers and students will find resources such as class schedules, grade books, and attendance sheets. Organize your family life with meal planners, checklists, and exercise logs. Each template is thoroughly researched, refined, and improved over time through feedback from thousands of users.</t>
+    <t>[Email]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="45" x14ac:knownFonts="1">
+  <fonts count="39" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Arial"/>
@@ -330,27 +268,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF1D2129"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="20"/>
-      <color theme="4" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="20"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="major"/>
@@ -445,31 +362,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1" tint="0.499984740745262"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1" tint="0.34998626667073579"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <color theme="1" tint="0.34998626667073579"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -917,7 +812,7 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -935,93 +830,64 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="44" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="44" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="44" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="44" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="44" applyFont="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="44" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="44" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="34" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="22" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="34" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="30" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="34" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="14" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="34" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="33" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="23" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
@@ -1052,10 +918,6 @@
     <xf numFmtId="43" fontId="20" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="20" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
@@ -1083,39 +945,38 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="44"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="44"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="45">
@@ -1244,118 +1105,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1640417</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>492919</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="Vertex42 logo">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7315200" y="123825"/>
-          <a:ext cx="1640417" cy="369094"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1905000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>523875</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="Vertex42 logo">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD7FCBBB-F986-458F-946D-D03E8EEEDCF6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="190500" y="95250"/>
-          <a:ext cx="1905000" cy="428625"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1624,636 +1373,490 @@
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:H38"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="12.625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="17.625" style="12" customWidth="1"/>
-    <col min="4" max="6" width="6.625" style="12" customWidth="1"/>
-    <col min="7" max="7" width="12.625" style="12" customWidth="1"/>
-    <col min="8" max="8" width="17.625" style="12" customWidth="1"/>
-    <col min="9" max="9" width="11.625" style="12" customWidth="1"/>
-    <col min="10" max="10" width="29" style="12" customWidth="1"/>
-    <col min="11" max="16384" width="9" style="12"/>
+    <col min="1" max="1" width="6.625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="12.625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="17.625" style="6" customWidth="1"/>
+    <col min="4" max="6" width="6.625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="12.625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="17.625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="11.625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="29" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="57" t="s">
+      <c r="F1" s="8"/>
+      <c r="G1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="57"/>
+      <c r="H1" s="45"/>
     </row>
     <row r="2" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>2</v>
+      <c r="A2" s="9" t="s">
+        <v>18</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="1"/>
       <c r="E2" s="3"/>
-      <c r="J2" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="K2" s="28"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="19"/>
     </row>
     <row r="3" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
-        <v>4</v>
+      <c r="A3" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="3"/>
-      <c r="J3" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="K3" s="24"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
     </row>
     <row r="4" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>6</v>
-      </c>
+      <c r="A4" s="9"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="1"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="59" t="s">
-        <v>7</v>
+      <c r="J4" s="25"/>
+    </row>
+    <row r="5" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>4</v>
       </c>
-      <c r="G4" s="59"/>
-      <c r="H4" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="J4" s="36"/>
-    </row>
-    <row r="5" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
       <c r="D5" s="1"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="60">
-        <v>2034</v>
+      <c r="F5" s="47" t="s">
+        <v>2</v>
       </c>
-      <c r="G5" s="60"/>
-      <c r="H5" s="34">
-        <v>43152</v>
+      <c r="G5" s="47"/>
+      <c r="H5" s="12" t="s">
+        <v>3</v>
       </c>
-      <c r="J5" s="36"/>
+      <c r="J5" s="25"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="F6" s="48">
+        <v>2034</v>
+      </c>
+      <c r="G6" s="48"/>
+      <c r="H6" s="23">
+        <v>43152</v>
+      </c>
       <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="62" t="s">
-        <v>9</v>
+      <c r="A7" s="3" t="s">
+        <v>6</v>
       </c>
-      <c r="B7" s="62"/>
-      <c r="C7" s="62"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="4"/>
-      <c r="F7" s="59" t="s">
-        <v>10</v>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="44"/>
+      <c r="J7" s="25"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
       </c>
-      <c r="G7" s="59"/>
-      <c r="H7" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="J7" s="36" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="3"/>
+      <c r="B8" s="1"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="61">
-        <v>564</v>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="20"/>
+      <c r="J8" s="25"/>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="3"/>
+      <c r="E9" s="4"/>
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>8</v>
       </c>
-      <c r="G8" s="61"/>
-      <c r="H8" s="29" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="40"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="31"/>
+      <c r="J11" s="26"/>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="41"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="35"/>
+      <c r="J12" s="25"/>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="41"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="35"/>
+      <c r="J13" s="25"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="41"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="35"/>
+      <c r="J14" s="25"/>
+    </row>
+    <row r="15" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="41"/>
+      <c r="B15" s="41"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="35"/>
+      <c r="J15" s="27"/>
+    </row>
+    <row r="16" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="41"/>
+      <c r="B16" s="41"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="35"/>
+      <c r="J16" s="25"/>
+    </row>
+    <row r="17" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="41"/>
+      <c r="B17" s="41"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="35"/>
+      <c r="J17" s="25"/>
+    </row>
+    <row r="18" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="41"/>
+      <c r="B18" s="41"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="35"/>
+      <c r="J18" s="25"/>
+    </row>
+    <row r="19" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="35"/>
+      <c r="J19" s="27"/>
+    </row>
+    <row r="20" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="41"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="35"/>
+      <c r="J20" s="27"/>
+    </row>
+    <row r="21" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="41"/>
+      <c r="B21" s="41"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="35"/>
+      <c r="J21" s="27"/>
+    </row>
+    <row r="22" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="41"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="35"/>
+      <c r="J22" s="27"/>
+    </row>
+    <row r="23" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="41"/>
+      <c r="B23" s="41"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="35"/>
+      <c r="J23" s="27"/>
+    </row>
+    <row r="24" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="41"/>
+      <c r="B24" s="41"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="35"/>
+      <c r="J24" s="27"/>
+    </row>
+    <row r="25" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="41"/>
+      <c r="B25" s="41"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="35"/>
+      <c r="J25" s="27"/>
+    </row>
+    <row r="26" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="41"/>
+      <c r="B26" s="41"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="35"/>
+      <c r="J26" s="27"/>
+    </row>
+    <row r="27" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="41"/>
+      <c r="B27" s="41"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="35"/>
+      <c r="J27" s="27"/>
+    </row>
+    <row r="28" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="41"/>
+      <c r="B28" s="41"/>
+      <c r="C28" s="41"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="35"/>
+      <c r="J28" s="27"/>
+    </row>
+    <row r="29" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="41"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="35"/>
+      <c r="J29" s="27"/>
+    </row>
+    <row r="30" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="42"/>
+      <c r="B30" s="42"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="39"/>
+      <c r="J30" s="27"/>
+    </row>
+    <row r="31" spans="1:10" s="7" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="51" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="51"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="51"/>
+      <c r="F31" s="52" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="52"/>
+      <c r="H31" s="22"/>
+      <c r="J31" s="25"/>
+    </row>
+    <row r="32" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="21"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="G32" s="52"/>
+      <c r="H32" s="54"/>
+      <c r="J32" s="25"/>
+    </row>
+    <row r="33" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="21"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="36"/>
-    </row>
-    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="J9" s="4"/>
-    </row>
-    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="J10" s="4"/>
-    </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="J11" s="37" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="J12" s="36" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="J13" s="36" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="J14" s="36" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="G15" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="H15" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="J15" s="38"/>
-    </row>
-    <row r="16" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="52"/>
-      <c r="B16" s="52"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="42"/>
-      <c r="J16" s="36"/>
-    </row>
-    <row r="17" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="53"/>
-      <c r="B17" s="53"/>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="46"/>
-      <c r="J17" s="36"/>
-    </row>
-    <row r="18" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="53"/>
-      <c r="B18" s="53"/>
-      <c r="C18" s="53"/>
-      <c r="D18" s="53"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="44"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="46"/>
-      <c r="J18" s="36" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="53"/>
-      <c r="B19" s="53"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="53"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="46"/>
-      <c r="J19" s="38"/>
-    </row>
-    <row r="20" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="53"/>
-      <c r="B20" s="53"/>
-      <c r="C20" s="53"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="44"/>
-      <c r="G20" s="45"/>
-      <c r="H20" s="46"/>
-      <c r="J20" s="38"/>
-    </row>
-    <row r="21" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="53"/>
-      <c r="B21" s="53"/>
-      <c r="C21" s="53"/>
-      <c r="D21" s="53"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="44"/>
-      <c r="G21" s="45"/>
-      <c r="H21" s="46"/>
-      <c r="J21" s="38"/>
-    </row>
-    <row r="22" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="53"/>
-      <c r="B22" s="53"/>
-      <c r="C22" s="53"/>
-      <c r="D22" s="53"/>
-      <c r="E22" s="43"/>
-      <c r="F22" s="44"/>
-      <c r="G22" s="45"/>
-      <c r="H22" s="46"/>
-      <c r="J22" s="38"/>
-    </row>
-    <row r="23" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="53"/>
-      <c r="B23" s="53"/>
-      <c r="C23" s="53"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="46"/>
-      <c r="J23" s="38"/>
-    </row>
-    <row r="24" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="53"/>
-      <c r="B24" s="53"/>
-      <c r="C24" s="53"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="44"/>
-      <c r="G24" s="45"/>
-      <c r="H24" s="46"/>
-      <c r="J24" s="38"/>
-    </row>
-    <row r="25" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="53"/>
-      <c r="B25" s="53"/>
-      <c r="C25" s="53"/>
-      <c r="D25" s="53"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="45"/>
-      <c r="H25" s="46"/>
-      <c r="J25" s="38"/>
-    </row>
-    <row r="26" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="53"/>
-      <c r="B26" s="53"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="44"/>
-      <c r="G26" s="45"/>
-      <c r="H26" s="46"/>
-      <c r="J26" s="38"/>
-    </row>
-    <row r="27" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="53"/>
-      <c r="B27" s="53"/>
-      <c r="C27" s="53"/>
-      <c r="D27" s="53"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="45"/>
-      <c r="H27" s="46"/>
-      <c r="J27" s="38"/>
-    </row>
-    <row r="28" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="53"/>
-      <c r="B28" s="53"/>
-      <c r="C28" s="53"/>
-      <c r="D28" s="53"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="44"/>
-      <c r="G28" s="45"/>
-      <c r="H28" s="46"/>
-      <c r="J28" s="38"/>
-    </row>
-    <row r="29" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="53"/>
-      <c r="B29" s="53"/>
-      <c r="C29" s="53"/>
-      <c r="D29" s="53"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="46"/>
-      <c r="J29" s="38"/>
-    </row>
-    <row r="30" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="54"/>
-      <c r="B30" s="54"/>
-      <c r="C30" s="54"/>
-      <c r="D30" s="54"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="49"/>
-      <c r="G30" s="50"/>
-      <c r="H30" s="51"/>
-      <c r="J30" s="38"/>
-    </row>
-    <row r="31" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="63" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31" s="63"/>
-      <c r="C31" s="63"/>
-      <c r="D31" s="63"/>
-      <c r="E31" s="63"/>
-      <c r="F31" s="64" t="s">
-        <v>27</v>
-      </c>
-      <c r="G31" s="64"/>
-      <c r="H31" s="32"/>
-      <c r="J31" s="36"/>
-    </row>
-    <row r="32" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="30"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="G32" s="64"/>
-      <c r="H32" s="33"/>
-      <c r="J32" s="36" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="30"/>
-      <c r="B33" s="17"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="G33" s="31"/>
-      <c r="H33" s="32"/>
-      <c r="J33" s="36"/>
-    </row>
-    <row r="34" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="30"/>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="56" t="s">
-        <v>31</v>
-      </c>
-      <c r="G34" s="56"/>
-      <c r="H34" s="21"/>
-      <c r="J34" s="36" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
+      <c r="G33" s="43"/>
+      <c r="H33" s="15"/>
+      <c r="J33" s="25"/>
+    </row>
+    <row r="34" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="J34" s="25"/>
+    </row>
+    <row r="35" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
-      <c r="J35" s="36" t="s">
-        <v>33</v>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="J35" s="25"/>
+    </row>
+    <row r="36" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="53" t="s">
+        <v>15</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="J36" s="36"/>
+      <c r="B36" s="53"/>
+      <c r="C36" s="53"/>
+      <c r="D36" s="53"/>
+      <c r="E36" s="53"/>
+      <c r="F36" s="53"/>
+      <c r="G36" s="53"/>
+      <c r="H36" s="53"/>
+      <c r="J36" s="27"/>
     </row>
     <row r="37" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="65" t="s">
-        <v>34</v>
+      <c r="A37" s="46" t="s">
+        <v>16</v>
       </c>
-      <c r="B37" s="65"/>
-      <c r="C37" s="65"/>
-      <c r="D37" s="65"/>
-      <c r="E37" s="65"/>
-      <c r="F37" s="65"/>
-      <c r="G37" s="65"/>
-      <c r="H37" s="65"/>
-      <c r="J37" s="38"/>
-    </row>
-    <row r="38" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="58" t="s">
-        <v>35</v>
-      </c>
-      <c r="B38" s="58"/>
-      <c r="C38" s="58"/>
-      <c r="D38" s="58"/>
-      <c r="E38" s="58"/>
-      <c r="F38" s="58"/>
-      <c r="G38" s="58"/>
-      <c r="H38" s="58"/>
-      <c r="J38" s="36" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J39" s="23"/>
+      <c r="B37" s="46"/>
+      <c r="C37" s="46"/>
+      <c r="D37" s="46"/>
+      <c r="E37" s="46"/>
+      <c r="F37" s="46"/>
+      <c r="G37" s="46"/>
+      <c r="H37" s="46"/>
+      <c r="J37" s="25"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J38" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="10">
     <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A38:H38"/>
-    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="A37:H37"/>
     <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="F8:G8"/>
-    <mergeCell ref="A7:C7"/>
     <mergeCell ref="A31:E31"/>
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="F32:G32"/>
-    <mergeCell ref="A37:H37"/>
+    <mergeCell ref="A36:H36"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"INVOICE,RECEIPT"</formula1>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="J3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-  </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" r:id="rId3"/>
-  <drawing r:id="rId4"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <tabColor theme="7" tint="0.59999389629810485"/>
-  </sheetPr>
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="78.625" style="6" customWidth="1"/>
-    <col min="2" max="16384" width="9" style="7"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:2" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="27"/>
-    </row>
-    <row r="3" spans="1:2" s="8" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="55" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="26"/>
-    </row>
-    <row r="4" spans="1:2" ht="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:2" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="60" x14ac:dyDescent="0.2">
-      <c r="A6" s="25" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="25"/>
-    </row>
-    <row r="8" spans="1:2" ht="75" x14ac:dyDescent="0.2">
-      <c r="A8" s="25" t="s">
-        <v>39</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
-  <drawing r:id="rId4"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2262,7 +1865,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="26" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac37c1753acd5e330d2062ccec26ea66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b340c7101c92c5120abd06486f94548" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2562,19 +2165,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71064D60-D5E2-4A90-940E-3D706FFDDDC0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85743C45-E9EB-4454-96EF-28ADC03776F7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -2582,7 +2193,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{327172A5-9D9E-46E2-A880-8096CFDFB9C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2603,6 +2214,18 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71064D60-D5E2-4A90-940E-3D706FFDDDC0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>